<commit_message>
test_sample line 23 mistake correction
</commit_message>
<xml_diff>
--- a/gpids.xlsx
+++ b/gpids.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,66 +459,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>GPID 2</t>
+          <t>5465564</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>GPNAME 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>GPID 3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>GPNAME 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>GPID 5</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>GPNAME 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>GPID 6</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>GPNAME 6</t>
+          <t>gp-partner 3</t>
         </is>
       </c>
     </row>

</xml_diff>